<commit_message>
updates for the new media table
</commit_message>
<xml_diff>
--- a/tools/excel-to-markdown/tests/SimpleTest.xlsx
+++ b/tools/excel-to-markdown/tests/SimpleTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrosenth/amas-tech-reports/tools/excel-to-markdown/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163B87DE-A46A-F340-979F-0BCCACE1DD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E678DBF6-A466-5042-9658-74071EEE8252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47060" yWindow="13880" windowWidth="27640" windowHeight="16940" xr2:uid="{A194B114-27F1-664A-95B8-857C49CE34E3}"/>
+    <workbookView xWindow="62700" yWindow="12040" windowWidth="27640" windowHeight="16940" xr2:uid="{A194B114-27F1-664A-95B8-857C49CE34E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Name of Standard/Specification</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>https://www.iso.org/standard/86831.html</t>
-  </si>
-  <si>
-    <t>Any, but focused on images</t>
   </si>
   <si>
     <t>JPEG Trust Part 2: Trust profiles catalog</t>
@@ -165,6 +162,35 @@
     <t>Content Provenance
 Trust and Authenticity
 Rights Declarations</t>
+  </si>
+  <si>
+    <t>Pub Date</t>
+  </si>
+  <si>
+    <t>TDM Reservation Protocol</t>
+  </si>
+  <si>
+    <t>Rights Declarations</t>
+  </si>
+  <si>
+    <t>W3C</t>
+  </si>
+  <si>
+    <t>TDMRep</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/ns/tdmrep/</t>
+  </si>
+  <si>
+    <t>Web pages
+EPUB
+PDF</t>
+  </si>
+  <si>
+    <t>This protocol provides guidelines for reserving content from text and data mining. It includes methods for creating and maintaining TDMRep files, which can be used to document the reservation of digital assets. This helps in ensuring that content is not used for data mining without the creator's consent.</t>
+  </si>
+  <si>
+    <t>Any (image focused)</t>
   </si>
 </sst>
 </file>
@@ -588,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91A65BA9-0B32-2E4D-AA83-8FDB48C10B0E}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,11 +628,12 @@
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="79" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" customWidth="1"/>
+    <col min="8" max="8" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="80" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="40" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -626,18 +653,21 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="80" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>9</v>
@@ -651,17 +681,20 @@
       <c r="F2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="5">
+        <v>2025</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="40" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>14</v>
@@ -675,17 +708,18 @@
       <c r="F3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="100" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>19</v>
@@ -699,79 +733,114 @@
       <c r="F4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="5">
+        <v>2025</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:9" ht="40" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" ht="100" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="B5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" ht="40" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="B6" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" ht="380" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" ht="380" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="5">
+        <v>2025</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>33</v>
+      <c r="I7" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="5" customFormat="1" ht="409.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>